<commit_message>
Ensure Sample names are cast as string when they are being read from the metadata spreadhseet
</commit_message>
<xml_diff>
--- a/tests/resources/metadata.xlsx
+++ b/tests/resources/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-submission/tests/resources/ftpboxes/eva-box-01/upload/john/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-submission/tests/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FBFAA0-93DD-0E46-A5D2-252A801C12B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B652153-D5FB-7B4F-A507-C2DAD8374641}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLEASE READ FIRST" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="Files" sheetId="10" r:id="rId10"/>
     <sheet name="CVs" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="764">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="763">
   <si>
     <t>PLEASE READ FIRST</t>
   </si>
@@ -1859,9 +1859,6 @@
   </si>
   <si>
     <t>It will be awesome as well</t>
-  </si>
-  <si>
-    <t>S1</t>
   </si>
   <si>
     <t>S2</t>
@@ -3026,6 +3023,21 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3035,23 +3047,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3431,8 +3428,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1">
-      <c r="A1" s="82"/>
-      <c r="B1" s="82"/>
+      <c r="A1" s="76"/>
+      <c r="B1" s="76"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -3441,10 +3438,10 @@
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="83"/>
+      <c r="B2" s="77"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -3453,10 +3450,10 @@
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" ht="19">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="78" t="s">
         <v>523</v>
       </c>
-      <c r="B3" s="84"/>
+      <c r="B3" s="78"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -3499,10 +3496,10 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A7" s="77" t="s">
+      <c r="A7" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="77"/>
+      <c r="B7" s="82"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -3511,8 +3508,8 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" s="9" customFormat="1">
-      <c r="A8" s="78"/>
-      <c r="B8" s="78"/>
+      <c r="A8" s="83"/>
+      <c r="B8" s="83"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
@@ -3543,10 +3540,10 @@
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" s="11" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="84" t="s">
         <v>518</v>
       </c>
-      <c r="B11" s="81"/>
+      <c r="B11" s="84"/>
     </row>
     <row r="12" spans="1:8" s="11" customFormat="1" ht="20">
       <c r="A12" s="35" t="s">
@@ -3599,28 +3596,28 @@
     </row>
     <row r="18" spans="1:2" s="11" customFormat="1"/>
     <row r="19" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A19" s="76" t="s">
+      <c r="A19" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="76"/>
+      <c r="B19" s="81"/>
     </row>
     <row r="20" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A20" s="76" t="s">
+      <c r="A20" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="76"/>
+      <c r="B20" s="81"/>
     </row>
     <row r="21" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A21" s="76" t="s">
+      <c r="A21" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="76"/>
+      <c r="B21" s="81"/>
     </row>
     <row r="22" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A22" s="76" t="s">
+      <c r="A22" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="76"/>
+      <c r="B22" s="81"/>
     </row>
     <row r="23" spans="1:2" s="4" customFormat="1">
       <c r="A23" s="14"/>
@@ -3629,11 +3626,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="qXS9mSszo6ZK4PVLf2a4mgrLN9LTYf+uHOdaWY7gal7eLQi1TYc4PKeNVhIGj1PsRxEc/Fk3JaqC7G3YqwmFZQ==" saltValue="v8qTKlsQPInt8A+7GIueog==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
@@ -3643,6 +3635,11 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -5411,7 +5408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -5452,16 +5449,16 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>759</v>
+      </c>
+      <c r="B2" t="s">
         <v>760</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="73" t="s">
         <v>761</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="D2" s="74" t="s">
         <v>762</v>
-      </c>
-      <c r="D2" s="74" t="s">
-        <v>763</v>
       </c>
       <c r="E2" t="s">
         <v>554</v>
@@ -7144,8 +7141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AT103"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -7454,11 +7451,11 @@
       <c r="A4" t="s">
         <v>558</v>
       </c>
-      <c r="F4" t="s">
-        <v>560</v>
+      <c r="F4">
+        <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="L4">
         <v>9606</v>
@@ -7472,10 +7469,10 @@
         <v>558</v>
       </c>
       <c r="F5" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="G5" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="L5">
         <v>9606</v>
@@ -7489,10 +7486,10 @@
         <v>558</v>
       </c>
       <c r="F6" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G6" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="L6">
         <v>9606</v>
@@ -7506,10 +7503,10 @@
         <v>558</v>
       </c>
       <c r="F7" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G7" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="L7">
         <v>9606</v>
@@ -7524,10 +7521,10 @@
         <v>558</v>
       </c>
       <c r="F8" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G8" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="L8">
         <v>9606</v>
@@ -7541,10 +7538,10 @@
         <v>558</v>
       </c>
       <c r="F9" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="G9" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="L9">
         <v>9606</v>
@@ -7558,10 +7555,10 @@
         <v>558</v>
       </c>
       <c r="F10" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G10" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="L10">
         <v>9606</v>
@@ -7575,10 +7572,10 @@
         <v>558</v>
       </c>
       <c r="F11" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="G11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="L11">
         <v>9606</v>
@@ -7592,10 +7589,10 @@
         <v>558</v>
       </c>
       <c r="F12" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="G12" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="L12">
         <v>9606</v>
@@ -7609,10 +7606,10 @@
         <v>558</v>
       </c>
       <c r="F13" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G13" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="L13">
         <v>9606</v>
@@ -7626,10 +7623,10 @@
         <v>558</v>
       </c>
       <c r="F14" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="G14" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="L14">
         <v>9606</v>
@@ -7643,10 +7640,10 @@
         <v>558</v>
       </c>
       <c r="F15" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="G15" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="L15">
         <v>9606</v>
@@ -7660,10 +7657,10 @@
         <v>558</v>
       </c>
       <c r="F16" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G16" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="L16">
         <v>9606</v>
@@ -7677,10 +7674,10 @@
         <v>558</v>
       </c>
       <c r="F17" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="G17" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="L17">
         <v>9606</v>
@@ -7694,10 +7691,10 @@
         <v>558</v>
       </c>
       <c r="F18" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="G18" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="L18">
         <v>9606</v>
@@ -7711,10 +7708,10 @@
         <v>558</v>
       </c>
       <c r="F19" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="G19" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="L19">
         <v>9606</v>
@@ -7728,10 +7725,10 @@
         <v>558</v>
       </c>
       <c r="F20" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="G20" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="L20">
         <v>9606</v>
@@ -7745,10 +7742,10 @@
         <v>558</v>
       </c>
       <c r="F21" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G21" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="L21">
         <v>9606</v>
@@ -7762,10 +7759,10 @@
         <v>558</v>
       </c>
       <c r="F22" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="G22" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="L22">
         <v>9606</v>
@@ -7779,10 +7776,10 @@
         <v>558</v>
       </c>
       <c r="F23" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G23" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="L23">
         <v>9606</v>
@@ -7796,10 +7793,10 @@
         <v>558</v>
       </c>
       <c r="F24" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="G24" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="L24">
         <v>9606</v>
@@ -7813,10 +7810,10 @@
         <v>558</v>
       </c>
       <c r="F25" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="G25" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="L25">
         <v>9606</v>
@@ -7830,10 +7827,10 @@
         <v>558</v>
       </c>
       <c r="F26" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="G26" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="L26">
         <v>9606</v>
@@ -7847,10 +7844,10 @@
         <v>558</v>
       </c>
       <c r="F27" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="G27" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="L27">
         <v>9606</v>
@@ -7864,10 +7861,10 @@
         <v>558</v>
       </c>
       <c r="F28" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="G28" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="L28">
         <v>9606</v>
@@ -7881,10 +7878,10 @@
         <v>558</v>
       </c>
       <c r="F29" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G29" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="L29">
         <v>9606</v>
@@ -7898,10 +7895,10 @@
         <v>558</v>
       </c>
       <c r="F30" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="G30" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="L30">
         <v>9606</v>
@@ -7915,10 +7912,10 @@
         <v>558</v>
       </c>
       <c r="F31" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G31" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="L31">
         <v>9606</v>
@@ -7932,10 +7929,10 @@
         <v>558</v>
       </c>
       <c r="F32" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="G32" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="L32">
         <v>9606</v>
@@ -7949,10 +7946,10 @@
         <v>558</v>
       </c>
       <c r="F33" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="G33" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="L33">
         <v>9606</v>
@@ -7966,10 +7963,10 @@
         <v>558</v>
       </c>
       <c r="F34" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="G34" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="L34">
         <v>9606</v>
@@ -7983,10 +7980,10 @@
         <v>558</v>
       </c>
       <c r="F35" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G35" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="L35">
         <v>9606</v>
@@ -8000,10 +7997,10 @@
         <v>558</v>
       </c>
       <c r="F36" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="G36" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="L36">
         <v>9606</v>
@@ -8017,10 +8014,10 @@
         <v>558</v>
       </c>
       <c r="F37" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="G37" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="L37">
         <v>9606</v>
@@ -8034,10 +8031,10 @@
         <v>558</v>
       </c>
       <c r="F38" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="G38" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="L38">
         <v>9606</v>
@@ -8051,10 +8048,10 @@
         <v>558</v>
       </c>
       <c r="F39" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="G39" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="L39">
         <v>9606</v>
@@ -8068,10 +8065,10 @@
         <v>558</v>
       </c>
       <c r="F40" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="G40" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="L40">
         <v>9606</v>
@@ -8085,10 +8082,10 @@
         <v>558</v>
       </c>
       <c r="F41" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G41" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="L41">
         <v>9606</v>
@@ -8102,10 +8099,10 @@
         <v>558</v>
       </c>
       <c r="F42" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G42" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="L42">
         <v>9606</v>
@@ -8119,10 +8116,10 @@
         <v>558</v>
       </c>
       <c r="F43" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G43" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="L43">
         <v>9606</v>
@@ -8136,10 +8133,10 @@
         <v>558</v>
       </c>
       <c r="F44" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="G44" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="L44">
         <v>9606</v>
@@ -8153,10 +8150,10 @@
         <v>558</v>
       </c>
       <c r="F45" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G45" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="L45">
         <v>9606</v>
@@ -8170,10 +8167,10 @@
         <v>558</v>
       </c>
       <c r="F46" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G46" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="L46">
         <v>9606</v>
@@ -8187,10 +8184,10 @@
         <v>558</v>
       </c>
       <c r="F47" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G47" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="L47">
         <v>9606</v>
@@ -8204,10 +8201,10 @@
         <v>558</v>
       </c>
       <c r="F48" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="G48" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="L48">
         <v>9606</v>
@@ -8221,10 +8218,10 @@
         <v>558</v>
       </c>
       <c r="F49" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="G49" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="L49">
         <v>9606</v>
@@ -8238,10 +8235,10 @@
         <v>558</v>
       </c>
       <c r="F50" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="G50" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="L50">
         <v>9606</v>
@@ -8255,10 +8252,10 @@
         <v>558</v>
       </c>
       <c r="F51" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G51" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="L51">
         <v>9606</v>
@@ -8272,10 +8269,10 @@
         <v>558</v>
       </c>
       <c r="F52" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G52" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="L52">
         <v>9606</v>
@@ -8289,10 +8286,10 @@
         <v>558</v>
       </c>
       <c r="F53" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="G53" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="L53">
         <v>9606</v>
@@ -8306,10 +8303,10 @@
         <v>558</v>
       </c>
       <c r="F54" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G54" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="L54">
         <v>9606</v>
@@ -8323,10 +8320,10 @@
         <v>558</v>
       </c>
       <c r="F55" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G55" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="L55">
         <v>9606</v>
@@ -8340,10 +8337,10 @@
         <v>558</v>
       </c>
       <c r="F56" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="G56" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="L56">
         <v>9606</v>
@@ -8357,10 +8354,10 @@
         <v>558</v>
       </c>
       <c r="F57" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="G57" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="L57">
         <v>9606</v>
@@ -8374,10 +8371,10 @@
         <v>558</v>
       </c>
       <c r="F58" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="G58" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="L58">
         <v>9606</v>
@@ -8391,10 +8388,10 @@
         <v>558</v>
       </c>
       <c r="F59" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G59" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="L59">
         <v>9606</v>
@@ -8408,10 +8405,10 @@
         <v>558</v>
       </c>
       <c r="F60" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="G60" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="L60">
         <v>9606</v>
@@ -8425,10 +8422,10 @@
         <v>558</v>
       </c>
       <c r="F61" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="G61" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="L61">
         <v>9606</v>
@@ -8442,10 +8439,10 @@
         <v>558</v>
       </c>
       <c r="F62" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="G62" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="L62">
         <v>9606</v>
@@ -8459,10 +8456,10 @@
         <v>558</v>
       </c>
       <c r="F63" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="G63" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="L63">
         <v>9606</v>
@@ -8476,10 +8473,10 @@
         <v>558</v>
       </c>
       <c r="F64" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="G64" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="L64">
         <v>9606</v>
@@ -8493,10 +8490,10 @@
         <v>558</v>
       </c>
       <c r="F65" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G65" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="L65">
         <v>9606</v>
@@ -8510,10 +8507,10 @@
         <v>558</v>
       </c>
       <c r="F66" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="G66" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="L66">
         <v>9606</v>
@@ -8527,10 +8524,10 @@
         <v>558</v>
       </c>
       <c r="F67" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G67" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="L67">
         <v>9606</v>
@@ -8544,10 +8541,10 @@
         <v>558</v>
       </c>
       <c r="F68" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="G68" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="L68">
         <v>9606</v>
@@ -8561,10 +8558,10 @@
         <v>558</v>
       </c>
       <c r="F69" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G69" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="L69">
         <v>9606</v>
@@ -8578,10 +8575,10 @@
         <v>558</v>
       </c>
       <c r="F70" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="G70" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="L70">
         <v>9606</v>
@@ -8595,10 +8592,10 @@
         <v>558</v>
       </c>
       <c r="F71" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G71" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="L71">
         <v>9606</v>
@@ -8612,10 +8609,10 @@
         <v>558</v>
       </c>
       <c r="F72" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G72" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="L72">
         <v>9606</v>
@@ -8629,10 +8626,10 @@
         <v>558</v>
       </c>
       <c r="F73" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="G73" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="L73">
         <v>9606</v>
@@ -8646,10 +8643,10 @@
         <v>558</v>
       </c>
       <c r="F74" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G74" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="L74">
         <v>9606</v>
@@ -8663,10 +8660,10 @@
         <v>558</v>
       </c>
       <c r="F75" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G75" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="L75">
         <v>9606</v>
@@ -8680,10 +8677,10 @@
         <v>558</v>
       </c>
       <c r="F76" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G76" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="L76">
         <v>9606</v>
@@ -8697,10 +8694,10 @@
         <v>558</v>
       </c>
       <c r="F77" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G77" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="L77">
         <v>9606</v>
@@ -8714,10 +8711,10 @@
         <v>558</v>
       </c>
       <c r="F78" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="G78" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="L78">
         <v>9606</v>
@@ -8731,10 +8728,10 @@
         <v>558</v>
       </c>
       <c r="F79" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G79" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="L79">
         <v>9606</v>
@@ -8748,10 +8745,10 @@
         <v>558</v>
       </c>
       <c r="F80" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G80" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="L80">
         <v>9606</v>
@@ -8765,10 +8762,10 @@
         <v>558</v>
       </c>
       <c r="F81" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="G81" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="L81">
         <v>9606</v>
@@ -8782,10 +8779,10 @@
         <v>558</v>
       </c>
       <c r="F82" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="G82" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="L82">
         <v>9606</v>
@@ -8799,10 +8796,10 @@
         <v>558</v>
       </c>
       <c r="F83" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="G83" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="L83">
         <v>9606</v>
@@ -8816,10 +8813,10 @@
         <v>558</v>
       </c>
       <c r="F84" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="G84" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="L84">
         <v>9606</v>
@@ -8833,10 +8830,10 @@
         <v>558</v>
       </c>
       <c r="F85" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="G85" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="L85">
         <v>9606</v>
@@ -8850,10 +8847,10 @@
         <v>558</v>
       </c>
       <c r="F86" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="G86" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="L86">
         <v>9606</v>
@@ -8867,10 +8864,10 @@
         <v>558</v>
       </c>
       <c r="F87" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="G87" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="L87">
         <v>9606</v>
@@ -8884,10 +8881,10 @@
         <v>558</v>
       </c>
       <c r="F88" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="G88" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="L88">
         <v>9606</v>
@@ -8901,10 +8898,10 @@
         <v>558</v>
       </c>
       <c r="F89" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="G89" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="L89">
         <v>9606</v>
@@ -8918,10 +8915,10 @@
         <v>558</v>
       </c>
       <c r="F90" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="G90" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="L90">
         <v>9606</v>
@@ -8935,10 +8932,10 @@
         <v>558</v>
       </c>
       <c r="F91" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G91" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="L91">
         <v>9606</v>
@@ -8952,10 +8949,10 @@
         <v>558</v>
       </c>
       <c r="F92" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="G92" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="L92">
         <v>9606</v>
@@ -8969,10 +8966,10 @@
         <v>558</v>
       </c>
       <c r="F93" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="G93" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="L93">
         <v>9606</v>
@@ -8986,10 +8983,10 @@
         <v>558</v>
       </c>
       <c r="F94" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="G94" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="L94">
         <v>9606</v>
@@ -9003,10 +9000,10 @@
         <v>558</v>
       </c>
       <c r="F95" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G95" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="L95">
         <v>9606</v>
@@ -9020,10 +9017,10 @@
         <v>558</v>
       </c>
       <c r="F96" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G96" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="L96">
         <v>9606</v>
@@ -9037,10 +9034,10 @@
         <v>558</v>
       </c>
       <c r="F97" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="G97" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="L97">
         <v>9606</v>
@@ -9054,10 +9051,10 @@
         <v>558</v>
       </c>
       <c r="F98" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G98" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="L98">
         <v>9606</v>
@@ -9071,10 +9068,10 @@
         <v>558</v>
       </c>
       <c r="F99" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="G99" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="L99">
         <v>9606</v>
@@ -9088,10 +9085,10 @@
         <v>558</v>
       </c>
       <c r="F100" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="G100" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="L100">
         <v>9606</v>
@@ -9105,10 +9102,10 @@
         <v>558</v>
       </c>
       <c r="F101" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="G101" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="L101">
         <v>9606</v>
@@ -9122,10 +9119,10 @@
         <v>558</v>
       </c>
       <c r="F102" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G102" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="L102">
         <v>9606</v>
@@ -9139,10 +9136,10 @@
         <v>558</v>
       </c>
       <c r="F103" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G103" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="L103">
         <v>9606</v>

</xml_diff>

<commit_message>
Trim leading and trailing whitespace when parsing the spreadsheet cells Added trailing and leading spaces in analysis alias of metadata
</commit_message>
<xml_diff>
--- a/tests/resources/metadata.xlsx
+++ b/tests/resources/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-submission/tests/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B652153-D5FB-7B4F-A507-C2DAD8374641}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C955EE7-B321-474C-B4D4-ECF212B3E316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40720" yWindow="500" windowWidth="23260" windowHeight="12580" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLEASE READ FIRST" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="Files" sheetId="10" r:id="rId10"/>
     <sheet name="CVs" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="763">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="764">
   <si>
     <t>PLEASE READ FIRST</t>
   </si>
@@ -2468,6 +2468,9 @@
   </si>
   <si>
     <t>john.doe@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  GAE     </t>
   </si>
 </sst>
 </file>
@@ -7142,7 +7145,7 @@
   <dimension ref="A1:AT103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -7449,7 +7452,7 @@
     </row>
     <row r="4" spans="1:46">
       <c r="A4" t="s">
-        <v>558</v>
+        <v>763</v>
       </c>
       <c r="F4">
         <v>1</v>

</xml_diff>